<commit_message>
add 200-tasks sa-tabu results
</commit_message>
<xml_diff>
--- a/docs/li_e_lim/Li e Lim - Java.xlsx
+++ b/docs/li_e_lim/Li e Lim - Java.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\aco-vrp-framework\docs\li_e_lim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2965AA0C-0E91-40A9-BDD7-0DA060EF8B3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94217443-A89E-4AC1-BD9C-F7920515B6DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21735" yWindow="-135" windowWidth="21870" windowHeight="13170" activeTab="2" xr2:uid="{6FDE03C4-3423-4D86-ADBA-4CA0DF9348DD}"/>
+    <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="3" xr2:uid="{6FDE03C4-3423-4D86-ADBA-4CA0DF9348DD}"/>
   </bookViews>
   <sheets>
     <sheet name="v1" sheetId="1" r:id="rId1"/>
     <sheet name="v2" sheetId="2" r:id="rId2"/>
-    <sheet name="v3" sheetId="3" r:id="rId3"/>
+    <sheet name="v3-100-tasks" sheetId="3" r:id="rId3"/>
+    <sheet name="v3-200-tasks" sheetId="4" r:id="rId4"/>
+    <sheet name="Folha2" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -102,8 +104,42 @@
 </comments>
 </file>
 
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>João Pedro</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{68BA1017-6779-4E52-8FDC-191805B65D10}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>João Pedro:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Usando rotinas do ALNS</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="128">
   <si>
     <t>LC101</t>
   </si>
@@ -304,6 +340,189 @@
   </si>
   <si>
     <t>Time (s)</t>
+  </si>
+  <si>
+    <t>lc1_2_3</t>
+  </si>
+  <si>
+    <t>lc1_2_8</t>
+  </si>
+  <si>
+    <t>lc1_2_10</t>
+  </si>
+  <si>
+    <t>lc2_2_3</t>
+  </si>
+  <si>
+    <t>lc2_2_6</t>
+  </si>
+  <si>
+    <t>lc2_2_7</t>
+  </si>
+  <si>
+    <t>lc2_2_9</t>
+  </si>
+  <si>
+    <t>lr1_2_3</t>
+  </si>
+  <si>
+    <t>lr1_2_4</t>
+  </si>
+  <si>
+    <t>lr1_2_6</t>
+  </si>
+  <si>
+    <t>lr1_2_7</t>
+  </si>
+  <si>
+    <t>lr1_2_8</t>
+  </si>
+  <si>
+    <t>lr1_2_9</t>
+  </si>
+  <si>
+    <t>lr1_2_10</t>
+  </si>
+  <si>
+    <t>lr2_2_1</t>
+  </si>
+  <si>
+    <t>lr2_2_2</t>
+  </si>
+  <si>
+    <t>lr2_2_4</t>
+  </si>
+  <si>
+    <t>lr2_2_5</t>
+  </si>
+  <si>
+    <t>lr2_2_6</t>
+  </si>
+  <si>
+    <t>lr2_2_7</t>
+  </si>
+  <si>
+    <t>lr2_2_8</t>
+  </si>
+  <si>
+    <t>lr2_2_9</t>
+  </si>
+  <si>
+    <t>lr2_2_10</t>
+  </si>
+  <si>
+    <t>lrc1_2_2</t>
+  </si>
+  <si>
+    <t>lrc1_2_3</t>
+  </si>
+  <si>
+    <t>lrc1_2_6</t>
+  </si>
+  <si>
+    <t>lrc1_2_7</t>
+  </si>
+  <si>
+    <t>lrc1_2_8</t>
+  </si>
+  <si>
+    <t>lrc1_2_9</t>
+  </si>
+  <si>
+    <t>lrc1_2_10</t>
+  </si>
+  <si>
+    <t>lrc2_2_1</t>
+  </si>
+  <si>
+    <t>lrc2_2_2</t>
+  </si>
+  <si>
+    <t>lrc2_2_3</t>
+  </si>
+  <si>
+    <t>lrc2_2_4</t>
+  </si>
+  <si>
+    <t>lrc2_2_6</t>
+  </si>
+  <si>
+    <t>lrc2_2_7</t>
+  </si>
+  <si>
+    <t>lrc2_2_8</t>
+  </si>
+  <si>
+    <t>lrc2_2_10</t>
+  </si>
+  <si>
+    <t>lc1_2_1</t>
+  </si>
+  <si>
+    <t>lc1_2_2</t>
+  </si>
+  <si>
+    <t>lc1_2_4</t>
+  </si>
+  <si>
+    <t>lc1_2_5</t>
+  </si>
+  <si>
+    <t>lc1_2_6</t>
+  </si>
+  <si>
+    <t>lc1_2_7</t>
+  </si>
+  <si>
+    <t>lc1_2_9</t>
+  </si>
+  <si>
+    <t>lc2_2_1</t>
+  </si>
+  <si>
+    <t>lc2_2_2</t>
+  </si>
+  <si>
+    <t>lc2_2_4</t>
+  </si>
+  <si>
+    <t>lc2_2_5</t>
+  </si>
+  <si>
+    <t>lc2_2_8</t>
+  </si>
+  <si>
+    <t>lc2_2_10</t>
+  </si>
+  <si>
+    <t>lr1_2_1</t>
+  </si>
+  <si>
+    <t>lr1_2_2</t>
+  </si>
+  <si>
+    <t>lr1_2_5</t>
+  </si>
+  <si>
+    <t>lr2_2_3</t>
+  </si>
+  <si>
+    <t>lrc1_2_1</t>
+  </si>
+  <si>
+    <t>lrc1_2_4</t>
+  </si>
+  <si>
+    <t>lrc1_2_5</t>
+  </si>
+  <si>
+    <t>lrc2_2_5</t>
+  </si>
+  <si>
+    <t>lrc2_2_9</t>
+  </si>
+  <si>
+    <t>Cpu Time (m)</t>
   </si>
 </sst>
 </file>
@@ -440,7 +659,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -466,6 +685,14 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="4" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -487,351 +714,25 @@
     <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="0" fillId="4" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="4" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percentagem" xfId="2" builtinId="5"/>
     <cellStyle name="Vírgula" xfId="1" builtinId="3"/>
   </cellStyles>
-  <dxfs count="45">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="12">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1279,31 +1180,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="12" t="s">
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="14" t="s">
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="13"/>
+      <c r="A2" s="17"/>
       <c r="B2" s="2" t="s">
         <v>41</v>
       </c>
@@ -4007,31 +3908,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="12" t="s">
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="14" t="s">
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" s="13"/>
+      <c r="A2" s="17"/>
       <c r="B2" s="2" t="s">
         <v>41</v>
       </c>
@@ -6892,8 +6793,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{522689FE-D32C-4FDE-A20E-61F329CB4E34}">
   <dimension ref="A1:P58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6901,39 +6802,39 @@
     <col min="1" max="1" width="10.44140625" style="1" customWidth="1"/>
     <col min="2" max="6" width="10.44140625" style="4" customWidth="1"/>
     <col min="7" max="11" width="10.44140625" style="5" customWidth="1"/>
-    <col min="12" max="12" width="10.44140625" style="20" customWidth="1"/>
-    <col min="13" max="13" width="10.44140625" style="21" customWidth="1"/>
+    <col min="12" max="12" width="10.44140625" style="13" customWidth="1"/>
+    <col min="13" max="13" width="10.44140625" style="14" customWidth="1"/>
     <col min="14" max="16" width="10.44140625" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="16" t="s">
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="14" t="s">
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
-      <c r="P1" s="15"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
+      <c r="P1" s="19"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A2" s="13"/>
+      <c r="A2" s="17"/>
       <c r="B2" s="2" t="s">
         <v>41</v>
       </c>
@@ -6964,10 +6865,10 @@
       <c r="K2" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="L2" s="18" t="s">
+      <c r="L2" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="M2" s="19" t="s">
+      <c r="M2" s="12" t="s">
         <v>42</v>
       </c>
       <c r="N2" s="7" t="s">
@@ -7014,11 +6915,11 @@
       <c r="K3" s="5">
         <v>2</v>
       </c>
-      <c r="L3" s="20">
+      <c r="L3" s="13">
         <f>ROUND(G3,2)/ROUND(B3,2)-1</f>
         <v>0</v>
       </c>
-      <c r="M3" s="20">
+      <c r="M3" s="13">
         <f>ROUND(H3,2)/ROUND(C3,2)-1</f>
         <v>0</v>
       </c>
@@ -7069,11 +6970,11 @@
       <c r="K4" s="5">
         <v>2</v>
       </c>
-      <c r="L4" s="20">
+      <c r="L4" s="13">
         <f t="shared" ref="L4:L58" si="0">ROUND(G4,2)/ROUND(B4,2)-1</f>
         <v>0</v>
       </c>
-      <c r="M4" s="20">
+      <c r="M4" s="13">
         <f t="shared" ref="M4:M58" si="1">ROUND(H4,2)/ROUND(C4,2)-1</f>
         <v>0</v>
       </c>
@@ -7124,11 +7025,11 @@
       <c r="K5" s="5">
         <v>4</v>
       </c>
-      <c r="L5" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M5" s="20">
+      <c r="L5" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M5" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -7179,11 +7080,11 @@
       <c r="K6" s="5">
         <v>17</v>
       </c>
-      <c r="L6" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M6" s="20">
+      <c r="L6" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M6" s="13">
         <f t="shared" si="1"/>
         <v>-2.2507105980625886E-3</v>
       </c>
@@ -7234,11 +7135,11 @@
       <c r="K7" s="5">
         <v>1</v>
       </c>
-      <c r="L7" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M7" s="20">
+      <c r="L7" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M7" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -7289,11 +7190,11 @@
       <c r="K8" s="5">
         <v>1</v>
       </c>
-      <c r="L8" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M8" s="20">
+      <c r="L8" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M8" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -7344,11 +7245,11 @@
       <c r="K9" s="5">
         <v>2</v>
       </c>
-      <c r="L9" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M9" s="20">
+      <c r="L9" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M9" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -7399,11 +7300,11 @@
       <c r="K10" s="5">
         <v>3</v>
       </c>
-      <c r="L10" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M10" s="20">
+      <c r="L10" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M10" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -7454,11 +7355,11 @@
       <c r="K11" s="5">
         <v>10</v>
       </c>
-      <c r="L11" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M11" s="20">
+      <c r="L11" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M11" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -7509,11 +7410,11 @@
       <c r="K12" s="5">
         <v>1</v>
       </c>
-      <c r="L12" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M12" s="20">
+      <c r="L12" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M12" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -7564,11 +7465,11 @@
       <c r="K13" s="5">
         <v>4</v>
       </c>
-      <c r="L13" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M13" s="20">
+      <c r="L13" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M13" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -7619,11 +7520,11 @@
       <c r="K14" s="5">
         <v>9</v>
       </c>
-      <c r="L14" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M14" s="20">
+      <c r="L14" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M14" s="13">
         <f t="shared" si="1"/>
         <v>9.58057244347299E-3</v>
       </c>
@@ -7674,11 +7575,11 @@
       <c r="K15" s="5">
         <v>28</v>
       </c>
-      <c r="L15" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M15" s="20">
+      <c r="L15" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M15" s="13">
         <f t="shared" si="1"/>
         <v>-9.6418965779709875E-4</v>
       </c>
@@ -7729,11 +7630,11 @@
       <c r="K16" s="5">
         <v>5</v>
       </c>
-      <c r="L16" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M16" s="20">
+      <c r="L16" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M16" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -7784,11 +7685,11 @@
       <c r="K17" s="5">
         <v>7</v>
       </c>
-      <c r="L17" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M17" s="20">
+      <c r="L17" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M17" s="13">
         <f t="shared" si="1"/>
         <v>6.3212628931672565E-3</v>
       </c>
@@ -7839,11 +7740,11 @@
       <c r="K18" s="5">
         <v>10</v>
       </c>
-      <c r="L18" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M18" s="20">
+      <c r="L18" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M18" s="13">
         <f t="shared" si="1"/>
         <v>1.1524928181679162E-2</v>
       </c>
@@ -7894,11 +7795,11 @@
       <c r="K19" s="5">
         <v>14</v>
       </c>
-      <c r="L19" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M19" s="20">
+      <c r="L19" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M19" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -7949,11 +7850,11 @@
       <c r="K20" s="5">
         <v>1</v>
       </c>
-      <c r="L20" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M20" s="20">
+      <c r="L20" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M20" s="13">
         <f t="shared" si="1"/>
         <v>1.2115484801178411E-5</v>
       </c>
@@ -8004,11 +7905,11 @@
       <c r="K21" s="5">
         <v>3</v>
       </c>
-      <c r="L21" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M21" s="20">
+      <c r="L21" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M21" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -8059,11 +7960,11 @@
       <c r="K22" s="5">
         <v>2</v>
       </c>
-      <c r="L22" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M22" s="20">
+      <c r="L22" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M22" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -8114,11 +8015,11 @@
       <c r="K23" s="5">
         <v>2</v>
       </c>
-      <c r="L23" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M23" s="20">
+      <c r="L23" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M23" s="13">
         <f t="shared" si="1"/>
         <v>3.4932257077728845E-3</v>
       </c>
@@ -8169,11 +8070,11 @@
       <c r="K24" s="5">
         <v>1</v>
       </c>
-      <c r="L24" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M24" s="20">
+      <c r="L24" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M24" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -8224,11 +8125,11 @@
       <c r="K25" s="5">
         <v>1</v>
       </c>
-      <c r="L25" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M25" s="20">
+      <c r="L25" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M25" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -8279,11 +8180,11 @@
       <c r="K26" s="5">
         <v>1</v>
       </c>
-      <c r="L26" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M26" s="20">
+      <c r="L26" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M26" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -8334,11 +8235,11 @@
       <c r="K27" s="5">
         <v>1</v>
       </c>
-      <c r="L27" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M27" s="20">
+      <c r="L27" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M27" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -8389,11 +8290,11 @@
       <c r="K28" s="5">
         <v>3</v>
       </c>
-      <c r="L28" s="20">
+      <c r="L28" s="13">
         <f t="shared" si="0"/>
         <v>9.0909090909090828E-2</v>
       </c>
-      <c r="M28" s="20">
+      <c r="M28" s="13">
         <f t="shared" si="1"/>
         <v>-1.9516758605117035E-3</v>
       </c>
@@ -8444,11 +8345,11 @@
       <c r="K29" s="5">
         <v>2</v>
       </c>
-      <c r="L29" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M29" s="20">
+      <c r="L29" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M29" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -8499,11 +8400,11 @@
       <c r="K30" s="5">
         <v>2</v>
       </c>
-      <c r="L30" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M30" s="20">
+      <c r="L30" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M30" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -8554,11 +8455,11 @@
       <c r="K31" s="5">
         <v>3</v>
       </c>
-      <c r="L31" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M31" s="20">
+      <c r="L31" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M31" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -8609,11 +8510,11 @@
       <c r="K32" s="5">
         <v>3</v>
       </c>
-      <c r="L32" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M32" s="20">
+      <c r="L32" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M32" s="13">
         <f t="shared" si="1"/>
         <v>-8.395050006329785E-3</v>
       </c>
@@ -8664,11 +8565,11 @@
       <c r="K33" s="5">
         <v>14</v>
       </c>
-      <c r="L33" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M33" s="20">
+      <c r="L33" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M33" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -8719,11 +8620,11 @@
       <c r="K34" s="5">
         <v>15</v>
       </c>
-      <c r="L34" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M34" s="20">
+      <c r="L34" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M34" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -8774,11 +8675,11 @@
       <c r="K35" s="5">
         <v>14</v>
       </c>
-      <c r="L35" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M35" s="20">
+      <c r="L35" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M35" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -8829,11 +8730,11 @@
       <c r="K36" s="5">
         <v>8</v>
       </c>
-      <c r="L36" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M36" s="20">
+      <c r="L36" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M36" s="13">
         <f t="shared" si="1"/>
         <v>1.6603100510426128E-3</v>
       </c>
@@ -8884,11 +8785,11 @@
       <c r="K37" s="5">
         <v>32</v>
       </c>
-      <c r="L37" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M37" s="20">
+      <c r="L37" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M37" s="13">
         <f t="shared" si="1"/>
         <v>4.7658405160848627E-3</v>
       </c>
@@ -8939,11 +8840,11 @@
       <c r="K38" s="5">
         <v>34</v>
       </c>
-      <c r="L38" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M38" s="20">
+      <c r="L38" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M38" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -8994,11 +8895,11 @@
       <c r="K39" s="5">
         <v>78</v>
       </c>
-      <c r="L39" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M39" s="20">
+      <c r="L39" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M39" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -9049,11 +8950,11 @@
       <c r="K40" s="5">
         <v>13</v>
       </c>
-      <c r="L40" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M40" s="20">
+      <c r="L40" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M40" s="13">
         <f t="shared" si="1"/>
         <v>2.8813830638707572E-3</v>
       </c>
@@ -9104,11 +9005,11 @@
       <c r="K41" s="5">
         <v>10</v>
       </c>
-      <c r="L41" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M41" s="20">
+      <c r="L41" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M41" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -9159,11 +9060,11 @@
       <c r="K42" s="5">
         <v>62</v>
       </c>
-      <c r="L42" s="20">
+      <c r="L42" s="13">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="M42" s="20">
+      <c r="M42" s="13">
         <f t="shared" si="1"/>
         <v>-4.4740245742616924E-2</v>
       </c>
@@ -9214,11 +9115,11 @@
       <c r="K43" s="5">
         <v>1</v>
       </c>
-      <c r="L43" s="20">
+      <c r="L43" s="13">
         <f t="shared" si="0"/>
         <v>7.1428571428571397E-2</v>
       </c>
-      <c r="M43" s="20">
+      <c r="M43" s="13">
         <f t="shared" si="1"/>
         <v>-3.2713014981272659E-3</v>
       </c>
@@ -9269,11 +9170,11 @@
       <c r="K44" s="5">
         <v>1</v>
       </c>
-      <c r="L44" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M44" s="20">
+      <c r="L44" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M44" s="13">
         <f t="shared" si="1"/>
         <v>2.2954174794538096E-2</v>
       </c>
@@ -9324,11 +9225,11 @@
       <c r="K45" s="5">
         <v>2</v>
       </c>
-      <c r="L45" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M45" s="20">
+      <c r="L45" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M45" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -9379,11 +9280,11 @@
       <c r="K46" s="5">
         <v>2</v>
       </c>
-      <c r="L46" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M46" s="20">
+      <c r="L46" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M46" s="13">
         <f t="shared" si="1"/>
         <v>5.3970223325061628E-3</v>
       </c>
@@ -9434,11 +9335,11 @@
       <c r="K47" s="5">
         <v>1</v>
       </c>
-      <c r="L47" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M47" s="20">
+      <c r="L47" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M47" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -9489,11 +9390,11 @@
       <c r="K48" s="5">
         <v>3</v>
       </c>
-      <c r="L48" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M48" s="20">
+      <c r="L48" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M48" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -9544,11 +9445,11 @@
       <c r="K49" s="5">
         <v>1</v>
       </c>
-      <c r="L49" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M49" s="20">
+      <c r="L49" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M49" s="13">
         <f t="shared" si="1"/>
         <v>5.6741047839694581E-3</v>
       </c>
@@ -9599,11 +9500,11 @@
       <c r="K50" s="5">
         <v>1</v>
       </c>
-      <c r="L50" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M50" s="20">
+      <c r="L50" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M50" s="13">
         <f t="shared" si="1"/>
         <v>-8.7110290338809904E-6</v>
       </c>
@@ -9654,11 +9555,11 @@
       <c r="K51" s="5">
         <v>3</v>
       </c>
-      <c r="L51" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M51" s="20">
+      <c r="L51" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M51" s="13">
         <f t="shared" si="1"/>
         <v>-4.1648513233852547E-2</v>
       </c>
@@ -9709,11 +9610,11 @@
       <c r="K52" s="5">
         <v>9</v>
       </c>
-      <c r="L52" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M52" s="20">
+      <c r="L52" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M52" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -9764,11 +9665,11 @@
       <c r="K53" s="5">
         <v>33</v>
       </c>
-      <c r="L53" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M53" s="20">
+      <c r="L53" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M53" s="13">
         <f t="shared" si="1"/>
         <v>8.0343779555032135E-3</v>
       </c>
@@ -9819,11 +9720,11 @@
       <c r="K54" s="5">
         <v>36</v>
       </c>
-      <c r="L54" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M54" s="20">
+      <c r="L54" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M54" s="13">
         <f t="shared" si="1"/>
         <v>-1.101742008746287E-2</v>
       </c>
@@ -9874,11 +9775,11 @@
       <c r="K55" s="5">
         <v>8</v>
       </c>
-      <c r="L55" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M55" s="20">
+      <c r="L55" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M55" s="13">
         <f t="shared" si="1"/>
         <v>2.6416833051758903E-3</v>
       </c>
@@ -9929,11 +9830,11 @@
       <c r="K56" s="5">
         <v>4</v>
       </c>
-      <c r="L56" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M56" s="20">
+      <c r="L56" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M56" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -9984,11 +9885,11 @@
       <c r="K57" s="5">
         <v>22</v>
       </c>
-      <c r="L57" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M57" s="20">
+      <c r="L57" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M57" s="13">
         <f t="shared" si="1"/>
         <v>-0.21789976133651545</v>
       </c>
@@ -10039,11 +9940,11 @@
       <c r="K58" s="5">
         <v>29</v>
       </c>
-      <c r="L58" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M58" s="20">
+      <c r="L58" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M58" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -10068,36 +9969,36 @@
     <mergeCell ref="G1:K1"/>
   </mergeCells>
   <conditionalFormatting sqref="L3:L58">
-    <cfRule type="cellIs" dxfId="14" priority="9" operator="lessThan">
+    <cfRule type="cellIs" dxfId="11" priority="9" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3:L58">
-    <cfRule type="cellIs" dxfId="13" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="8" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M3:M58">
-    <cfRule type="cellIs" dxfId="12" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="6" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="8" priority="7" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N3:N58">
-    <cfRule type="cellIs" dxfId="10" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O3:O58">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10108,4 +10009,2466 @@
   </ignoredErrors>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBE9A944-D29F-4B55-959D-80A528CF29DA}">
+  <dimension ref="A1:K62"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="L54" sqref="L54"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="9" max="10" width="8.88671875" style="28"/>
+    <col min="11" max="11" width="12.44140625" style="24" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="15"/>
+      <c r="D1" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="17"/>
+      <c r="B2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="I2" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="J2" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B3" s="25">
+        <v>20</v>
+      </c>
+      <c r="C3" s="25">
+        <v>2704.57</v>
+      </c>
+      <c r="D3">
+        <v>20</v>
+      </c>
+      <c r="E3">
+        <v>2704.56776633047</v>
+      </c>
+      <c r="H3" s="5">
+        <v>11</v>
+      </c>
+      <c r="I3" s="27">
+        <f>ROUND(D3,2)/ROUND(B3,2)-1</f>
+        <v>0</v>
+      </c>
+      <c r="J3" s="27">
+        <f>ROUND(E3,2)/ROUND(C3,2)-1</f>
+        <v>0</v>
+      </c>
+      <c r="K3" s="23">
+        <f>H3/60</f>
+        <v>0.18333333333333332</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B4" s="25">
+        <v>19</v>
+      </c>
+      <c r="C4" s="25">
+        <v>2764.56</v>
+      </c>
+      <c r="D4">
+        <v>19</v>
+      </c>
+      <c r="E4">
+        <v>2769.5454368032601</v>
+      </c>
+      <c r="F4">
+        <v>21156.4932806139</v>
+      </c>
+      <c r="G4">
+        <v>386.94784381063499</v>
+      </c>
+      <c r="H4">
+        <v>17</v>
+      </c>
+      <c r="I4" s="27">
+        <f t="shared" ref="I4:I62" si="0">ROUND(D4,2)/ROUND(B4,2)-1</f>
+        <v>0</v>
+      </c>
+      <c r="J4" s="27">
+        <f t="shared" ref="J4:J62" si="1">ROUND(E4,2)/ROUND(C4,2)-1</f>
+        <v>1.8049888589866114E-3</v>
+      </c>
+      <c r="K4" s="23">
+        <f t="shared" ref="K4:K62" si="2">H4/60</f>
+        <v>0.28333333333333333</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" s="25">
+        <v>17</v>
+      </c>
+      <c r="C5" s="25">
+        <v>3127.78</v>
+      </c>
+      <c r="D5">
+        <v>18</v>
+      </c>
+      <c r="E5">
+        <v>2772.1821743258902</v>
+      </c>
+      <c r="F5">
+        <v>21219.503578425501</v>
+      </c>
+      <c r="G5">
+        <v>447.32140409966303</v>
+      </c>
+      <c r="H5">
+        <v>26</v>
+      </c>
+      <c r="I5" s="27">
+        <f t="shared" si="0"/>
+        <v>5.8823529411764719E-2</v>
+      </c>
+      <c r="J5" s="27">
+        <f t="shared" si="1"/>
+        <v>-0.11369086061040112</v>
+      </c>
+      <c r="K5" s="23">
+        <f t="shared" si="2"/>
+        <v>0.43333333333333335</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>107</v>
+      </c>
+      <c r="B6" s="25">
+        <v>17</v>
+      </c>
+      <c r="C6" s="25">
+        <v>2693.41</v>
+      </c>
+      <c r="D6">
+        <v>17</v>
+      </c>
+      <c r="E6">
+        <v>2693.5900854821698</v>
+      </c>
+      <c r="F6">
+        <v>21370.914789898601</v>
+      </c>
+      <c r="G6">
+        <v>677.32470441650901</v>
+      </c>
+      <c r="H6">
+        <v>174</v>
+      </c>
+      <c r="I6" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J6" s="27">
+        <f t="shared" si="1"/>
+        <v>6.6829780835497843E-5</v>
+      </c>
+      <c r="K6" s="23">
+        <f t="shared" si="2"/>
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>108</v>
+      </c>
+      <c r="B7" s="25">
+        <v>20</v>
+      </c>
+      <c r="C7" s="25">
+        <v>2702.05</v>
+      </c>
+      <c r="D7">
+        <v>20</v>
+      </c>
+      <c r="E7">
+        <v>2702.04876554162</v>
+      </c>
+      <c r="F7">
+        <v>20771.366824680201</v>
+      </c>
+      <c r="G7">
+        <v>69.318059138638404</v>
+      </c>
+      <c r="H7">
+        <v>12</v>
+      </c>
+      <c r="I7" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J7" s="27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K7" s="23">
+        <f t="shared" si="2"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>109</v>
+      </c>
+      <c r="B8" s="25">
+        <v>20</v>
+      </c>
+      <c r="C8" s="25">
+        <v>2701.04</v>
+      </c>
+      <c r="D8">
+        <v>20</v>
+      </c>
+      <c r="E8">
+        <v>2701.0353881583801</v>
+      </c>
+      <c r="F8">
+        <v>20820.747896021501</v>
+      </c>
+      <c r="G8">
+        <v>119.712507863174</v>
+      </c>
+      <c r="H8">
+        <v>12</v>
+      </c>
+      <c r="I8" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J8" s="27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K8" s="23">
+        <f t="shared" si="2"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>110</v>
+      </c>
+      <c r="B9" s="25">
+        <v>20</v>
+      </c>
+      <c r="C9" s="25">
+        <v>2701.04</v>
+      </c>
+      <c r="D9">
+        <v>20</v>
+      </c>
+      <c r="E9">
+        <v>2701.0353881583801</v>
+      </c>
+      <c r="F9">
+        <v>20708.353447296999</v>
+      </c>
+      <c r="G9">
+        <v>7.3180591386384304</v>
+      </c>
+      <c r="H9">
+        <v>17</v>
+      </c>
+      <c r="I9" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J9" s="27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K9" s="23">
+        <f t="shared" si="2"/>
+        <v>0.28333333333333333</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" s="25">
+        <v>19</v>
+      </c>
+      <c r="C10" s="25">
+        <v>3354.27</v>
+      </c>
+      <c r="D10">
+        <v>20</v>
+      </c>
+      <c r="E10">
+        <v>2689.8330608342199</v>
+      </c>
+      <c r="F10">
+        <v>20869.954372567099</v>
+      </c>
+      <c r="G10">
+        <v>180.121311732885</v>
+      </c>
+      <c r="H10">
+        <v>26</v>
+      </c>
+      <c r="I10" s="27">
+        <f t="shared" si="0"/>
+        <v>5.2631578947368363E-2</v>
+      </c>
+      <c r="J10" s="27">
+        <f t="shared" si="1"/>
+        <v>-0.19808781046248514</v>
+      </c>
+      <c r="K10" s="23">
+        <f t="shared" si="2"/>
+        <v>0.43333333333333335</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>111</v>
+      </c>
+      <c r="B11" s="25">
+        <v>18</v>
+      </c>
+      <c r="C11" s="25">
+        <v>2724.24</v>
+      </c>
+      <c r="D11">
+        <v>18</v>
+      </c>
+      <c r="E11">
+        <v>2724.2352747165701</v>
+      </c>
+      <c r="F11">
+        <v>20748.403467168198</v>
+      </c>
+      <c r="G11">
+        <v>24.168192451719499</v>
+      </c>
+      <c r="H11">
+        <v>28</v>
+      </c>
+      <c r="I11" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J11" s="27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K11" s="23">
+        <f t="shared" si="2"/>
+        <v>0.46666666666666667</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>69</v>
+      </c>
+      <c r="B12" s="25">
+        <v>17</v>
+      </c>
+      <c r="C12" s="25">
+        <v>2942.13</v>
+      </c>
+      <c r="D12">
+        <v>18</v>
+      </c>
+      <c r="E12">
+        <v>2741.5594825267599</v>
+      </c>
+      <c r="F12">
+        <v>21066.408152510401</v>
+      </c>
+      <c r="G12">
+        <v>324.84866998371899</v>
+      </c>
+      <c r="H12">
+        <v>46</v>
+      </c>
+      <c r="I12" s="27">
+        <f t="shared" si="0"/>
+        <v>5.8823529411764719E-2</v>
+      </c>
+      <c r="J12" s="27">
+        <f t="shared" si="1"/>
+        <v>-6.817169873527007E-2</v>
+      </c>
+      <c r="K12" s="23">
+        <f t="shared" si="2"/>
+        <v>0.76666666666666672</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>112</v>
+      </c>
+      <c r="B13" s="25">
+        <v>6</v>
+      </c>
+      <c r="C13" s="25">
+        <v>1931.44</v>
+      </c>
+      <c r="D13">
+        <v>6</v>
+      </c>
+      <c r="E13">
+        <v>1931.4425029392</v>
+      </c>
+      <c r="F13">
+        <v>19941.4009083604</v>
+      </c>
+      <c r="G13">
+        <v>9.9584054212077007</v>
+      </c>
+      <c r="H13">
+        <v>8</v>
+      </c>
+      <c r="I13" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J13" s="27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K13" s="23">
+        <f t="shared" si="2"/>
+        <v>0.13333333333333333</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>113</v>
+      </c>
+      <c r="B14" s="25">
+        <v>6</v>
+      </c>
+      <c r="C14" s="25">
+        <v>1881.4</v>
+      </c>
+      <c r="D14">
+        <v>6</v>
+      </c>
+      <c r="E14">
+        <v>1881.4023058569001</v>
+      </c>
+      <c r="F14">
+        <v>20707.055443732501</v>
+      </c>
+      <c r="G14">
+        <v>825.65313787568004</v>
+      </c>
+      <c r="H14">
+        <v>33</v>
+      </c>
+      <c r="I14" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J14" s="27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K14" s="23">
+        <f t="shared" si="2"/>
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>70</v>
+      </c>
+      <c r="B15" s="25">
+        <v>6</v>
+      </c>
+      <c r="C15" s="25">
+        <v>1844.33</v>
+      </c>
+      <c r="D15">
+        <v>6</v>
+      </c>
+      <c r="E15">
+        <v>1848.3748619683199</v>
+      </c>
+      <c r="F15">
+        <v>20590.156854520901</v>
+      </c>
+      <c r="G15">
+        <v>741.78199255258096</v>
+      </c>
+      <c r="H15">
+        <v>70</v>
+      </c>
+      <c r="I15" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J15" s="27">
+        <f t="shared" si="1"/>
+        <v>2.1904973621857948E-3</v>
+      </c>
+      <c r="K15" s="23">
+        <f t="shared" si="2"/>
+        <v>1.1666666666666667</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>114</v>
+      </c>
+      <c r="B16" s="25">
+        <v>6</v>
+      </c>
+      <c r="C16" s="25">
+        <v>1767.12</v>
+      </c>
+      <c r="D16">
+        <v>6</v>
+      </c>
+      <c r="E16">
+        <v>1767.1183001071799</v>
+      </c>
+      <c r="F16">
+        <v>20838.5837675982</v>
+      </c>
+      <c r="G16">
+        <v>1071.4654674910701</v>
+      </c>
+      <c r="H16">
+        <v>204</v>
+      </c>
+      <c r="I16" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J16" s="27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K16" s="23">
+        <f t="shared" si="2"/>
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>115</v>
+      </c>
+      <c r="B17" s="25">
+        <v>6</v>
+      </c>
+      <c r="C17" s="25">
+        <v>1891.21</v>
+      </c>
+      <c r="D17">
+        <v>6</v>
+      </c>
+      <c r="E17">
+        <v>1891.2089948477401</v>
+      </c>
+      <c r="F17">
+        <v>20011.211350207799</v>
+      </c>
+      <c r="G17">
+        <v>120.00235536015001</v>
+      </c>
+      <c r="H17">
+        <v>25</v>
+      </c>
+      <c r="I17" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J17" s="27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K17" s="23">
+        <f t="shared" si="2"/>
+        <v>0.41666666666666669</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>71</v>
+      </c>
+      <c r="B18" s="25">
+        <v>6</v>
+      </c>
+      <c r="C18" s="25">
+        <v>1857.78</v>
+      </c>
+      <c r="D18">
+        <v>6</v>
+      </c>
+      <c r="E18">
+        <v>1858.25368731858</v>
+      </c>
+      <c r="F18">
+        <v>19937.750907396901</v>
+      </c>
+      <c r="G18">
+        <v>79.4972200783251</v>
+      </c>
+      <c r="H18">
+        <v>40</v>
+      </c>
+      <c r="I18" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J18" s="27">
+        <f t="shared" si="1"/>
+        <v>2.5299012800217291E-4</v>
+      </c>
+      <c r="K18" s="23">
+        <f t="shared" si="2"/>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19" s="25">
+        <v>6</v>
+      </c>
+      <c r="C19" s="25">
+        <v>1850.13</v>
+      </c>
+      <c r="D19">
+        <v>6</v>
+      </c>
+      <c r="E19">
+        <v>1850.6328975398901</v>
+      </c>
+      <c r="F19">
+        <v>19984.9150902451</v>
+      </c>
+      <c r="G19">
+        <v>134.282192705245</v>
+      </c>
+      <c r="H19">
+        <v>34</v>
+      </c>
+      <c r="I19" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J19" s="27">
+        <f t="shared" si="1"/>
+        <v>2.7025127963975493E-4</v>
+      </c>
+      <c r="K19" s="23">
+        <f t="shared" si="2"/>
+        <v>0.56666666666666665</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>116</v>
+      </c>
+      <c r="B20" s="25">
+        <v>6</v>
+      </c>
+      <c r="C20" s="25">
+        <v>1824.34</v>
+      </c>
+      <c r="D20">
+        <v>6</v>
+      </c>
+      <c r="E20">
+        <v>1826.02396737054</v>
+      </c>
+      <c r="F20">
+        <v>19894.448280697401</v>
+      </c>
+      <c r="G20">
+        <v>68.424313326942993</v>
+      </c>
+      <c r="H20">
+        <v>96</v>
+      </c>
+      <c r="I20" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J20" s="27">
+        <f t="shared" si="1"/>
+        <v>9.2088097613385322E-4</v>
+      </c>
+      <c r="K20" s="23">
+        <f t="shared" si="2"/>
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>73</v>
+      </c>
+      <c r="B21" s="25">
+        <v>6</v>
+      </c>
+      <c r="C21" s="25">
+        <v>1854.21</v>
+      </c>
+      <c r="D21">
+        <v>6</v>
+      </c>
+      <c r="E21">
+        <v>1870.3058405054801</v>
+      </c>
+      <c r="F21">
+        <v>20032.473651313001</v>
+      </c>
+      <c r="G21">
+        <v>162.16781080752</v>
+      </c>
+      <c r="H21">
+        <v>41</v>
+      </c>
+      <c r="I21" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J21" s="27">
+        <f t="shared" si="1"/>
+        <v>8.6829431402051238E-3</v>
+      </c>
+      <c r="K21" s="23">
+        <f t="shared" si="2"/>
+        <v>0.68333333333333335</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>117</v>
+      </c>
+      <c r="B22" s="25">
+        <v>6</v>
+      </c>
+      <c r="C22" s="25">
+        <v>1817.45</v>
+      </c>
+      <c r="D22">
+        <v>6</v>
+      </c>
+      <c r="E22">
+        <v>1817.92974627031</v>
+      </c>
+      <c r="F22">
+        <v>20230.037375181098</v>
+      </c>
+      <c r="G22">
+        <v>412.10762891085398</v>
+      </c>
+      <c r="H22">
+        <v>258</v>
+      </c>
+      <c r="I22" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J22" s="27">
+        <f t="shared" si="1"/>
+        <v>2.6410630278683733E-4</v>
+      </c>
+      <c r="K22" s="23">
+        <f t="shared" si="2"/>
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>118</v>
+      </c>
+      <c r="B23" s="25">
+        <v>20</v>
+      </c>
+      <c r="C23" s="25">
+        <v>4819.12</v>
+      </c>
+      <c r="D23">
+        <v>21</v>
+      </c>
+      <c r="E23">
+        <v>4900.33067317118</v>
+      </c>
+      <c r="F23">
+        <v>11289.2989408372</v>
+      </c>
+      <c r="G23">
+        <v>4388.9682676660104</v>
+      </c>
+      <c r="H23">
+        <v>10</v>
+      </c>
+      <c r="I23" s="27">
+        <f t="shared" si="0"/>
+        <v>5.0000000000000044E-2</v>
+      </c>
+      <c r="J23" s="27">
+        <f t="shared" si="1"/>
+        <v>1.6851624362954176E-2</v>
+      </c>
+      <c r="K23" s="23">
+        <f t="shared" si="2"/>
+        <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>119</v>
+      </c>
+      <c r="B24" s="25">
+        <v>17</v>
+      </c>
+      <c r="C24" s="25">
+        <v>4621.21</v>
+      </c>
+      <c r="D24">
+        <v>18</v>
+      </c>
+      <c r="E24">
+        <v>4295.1179680109099</v>
+      </c>
+      <c r="F24">
+        <v>9745.2256121999799</v>
+      </c>
+      <c r="G24">
+        <v>3450.10764418906</v>
+      </c>
+      <c r="H24">
+        <v>29</v>
+      </c>
+      <c r="I24" s="27">
+        <f t="shared" si="0"/>
+        <v>5.8823529411764719E-2</v>
+      </c>
+      <c r="J24" s="27">
+        <f t="shared" si="1"/>
+        <v>-7.0563770094845268E-2</v>
+      </c>
+      <c r="K24" s="23">
+        <f t="shared" si="2"/>
+        <v>0.48333333333333334</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>74</v>
+      </c>
+      <c r="B25" s="25">
+        <v>14</v>
+      </c>
+      <c r="C25" s="25">
+        <v>4402.38</v>
+      </c>
+      <c r="D25">
+        <v>15</v>
+      </c>
+      <c r="E25">
+        <v>3741.70090047546</v>
+      </c>
+      <c r="F25">
+        <v>8205.2768131520497</v>
+      </c>
+      <c r="G25">
+        <v>2463.5759126765902</v>
+      </c>
+      <c r="H25">
+        <v>111</v>
+      </c>
+      <c r="I25" s="27">
+        <f t="shared" si="0"/>
+        <v>7.1428571428571397E-2</v>
+      </c>
+      <c r="J25" s="27">
+        <f t="shared" si="1"/>
+        <v>-0.15007336940473115</v>
+      </c>
+      <c r="K25" s="23">
+        <f t="shared" si="2"/>
+        <v>1.85</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>75</v>
+      </c>
+      <c r="B26" s="25">
+        <v>10</v>
+      </c>
+      <c r="C26" s="25">
+        <v>3027.06</v>
+      </c>
+      <c r="D26">
+        <v>11</v>
+      </c>
+      <c r="E26">
+        <v>3005.4055270899298</v>
+      </c>
+      <c r="F26">
+        <v>6263.8555621940104</v>
+      </c>
+      <c r="G26">
+        <v>1258.4500351040699</v>
+      </c>
+      <c r="H26">
+        <v>154</v>
+      </c>
+      <c r="I26" s="27">
+        <f t="shared" si="0"/>
+        <v>0.10000000000000009</v>
+      </c>
+      <c r="J26" s="27">
+        <f t="shared" si="1"/>
+        <v>-7.1521542354627821E-3</v>
+      </c>
+      <c r="K26" s="23">
+        <f t="shared" si="2"/>
+        <v>2.5666666666666669</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>120</v>
+      </c>
+      <c r="B27" s="25">
+        <v>16</v>
+      </c>
+      <c r="C27" s="25">
+        <v>4760.18</v>
+      </c>
+      <c r="D27">
+        <v>17</v>
+      </c>
+      <c r="E27">
+        <v>4331.1409819792398</v>
+      </c>
+      <c r="F27">
+        <v>9054.7488208763007</v>
+      </c>
+      <c r="G27">
+        <v>2723.60783889705</v>
+      </c>
+      <c r="H27">
+        <v>18</v>
+      </c>
+      <c r="I27" s="27">
+        <f t="shared" si="0"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="J27" s="27">
+        <f t="shared" si="1"/>
+        <v>-9.0131045464667325E-2</v>
+      </c>
+      <c r="K27" s="23">
+        <f t="shared" si="2"/>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>76</v>
+      </c>
+      <c r="B28" s="25">
+        <v>13</v>
+      </c>
+      <c r="C28" s="25">
+        <v>4800.9399999999996</v>
+      </c>
+      <c r="D28">
+        <v>15</v>
+      </c>
+      <c r="E28">
+        <v>4095.5190525462499</v>
+      </c>
+      <c r="F28">
+        <v>8237.1045719301092</v>
+      </c>
+      <c r="G28">
+        <v>2141.5855193838602</v>
+      </c>
+      <c r="H28">
+        <v>60</v>
+      </c>
+      <c r="I28" s="27">
+        <f t="shared" si="0"/>
+        <v>0.15384615384615374</v>
+      </c>
+      <c r="J28" s="27">
+        <f t="shared" si="1"/>
+        <v>-0.14693372547876038</v>
+      </c>
+      <c r="K28" s="23">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>77</v>
+      </c>
+      <c r="B29" s="25">
+        <v>12</v>
+      </c>
+      <c r="C29" s="25">
+        <v>3543.36</v>
+      </c>
+      <c r="D29">
+        <v>13</v>
+      </c>
+      <c r="E29">
+        <v>3555.2510508014402</v>
+      </c>
+      <c r="F29">
+        <v>6731.2359269573499</v>
+      </c>
+      <c r="G29">
+        <v>1175.9848761559099</v>
+      </c>
+      <c r="H29">
+        <v>71</v>
+      </c>
+      <c r="I29" s="27">
+        <f t="shared" si="0"/>
+        <v>8.3333333333333259E-2</v>
+      </c>
+      <c r="J29" s="27">
+        <f t="shared" si="1"/>
+        <v>3.3555721123452731E-3</v>
+      </c>
+      <c r="K29" s="23">
+        <f t="shared" si="2"/>
+        <v>1.1833333333333333</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>78</v>
+      </c>
+      <c r="B30" s="25">
+        <v>9</v>
+      </c>
+      <c r="C30" s="25">
+        <v>2759.32</v>
+      </c>
+      <c r="D30">
+        <v>9</v>
+      </c>
+      <c r="E30">
+        <v>2832.1150237260199</v>
+      </c>
+      <c r="F30">
+        <v>5255.61761753683</v>
+      </c>
+      <c r="G30">
+        <v>423.50259381081202</v>
+      </c>
+      <c r="H30">
+        <v>50</v>
+      </c>
+      <c r="I30" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J30" s="27">
+        <f t="shared" si="1"/>
+        <v>2.638331183045084E-2</v>
+      </c>
+      <c r="K30" s="23">
+        <f t="shared" si="2"/>
+        <v>0.83333333333333337</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>79</v>
+      </c>
+      <c r="B31" s="25">
+        <v>13</v>
+      </c>
+      <c r="C31" s="25">
+        <v>5050.75</v>
+      </c>
+      <c r="D31">
+        <v>15</v>
+      </c>
+      <c r="E31">
+        <v>4138.6713037196896</v>
+      </c>
+      <c r="F31">
+        <v>7920.5572320057299</v>
+      </c>
+      <c r="G31">
+        <v>1781.8859282860301</v>
+      </c>
+      <c r="H31">
+        <v>26</v>
+      </c>
+      <c r="I31" s="27">
+        <f t="shared" si="0"/>
+        <v>0.15384615384615374</v>
+      </c>
+      <c r="J31" s="27">
+        <f t="shared" si="1"/>
+        <v>-0.1805830817205365</v>
+      </c>
+      <c r="K31" s="23">
+        <f t="shared" si="2"/>
+        <v>0.43333333333333335</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>80</v>
+      </c>
+      <c r="B32" s="25">
+        <v>11</v>
+      </c>
+      <c r="C32" s="25">
+        <v>3664.08</v>
+      </c>
+      <c r="D32">
+        <v>12</v>
+      </c>
+      <c r="E32">
+        <v>3633.2991578526198</v>
+      </c>
+      <c r="F32">
+        <v>6400.2610521738497</v>
+      </c>
+      <c r="G32">
+        <v>766.96189432123003</v>
+      </c>
+      <c r="H32">
+        <v>23</v>
+      </c>
+      <c r="I32" s="27">
+        <f t="shared" si="0"/>
+        <v>9.0909090909090828E-2</v>
+      </c>
+      <c r="J32" s="27">
+        <f t="shared" si="1"/>
+        <v>-8.400471605423343E-3</v>
+      </c>
+      <c r="K32" s="23">
+        <f t="shared" si="2"/>
+        <v>0.38333333333333336</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>81</v>
+      </c>
+      <c r="B33" s="25">
+        <v>5</v>
+      </c>
+      <c r="C33" s="25">
+        <v>4073.1</v>
+      </c>
+      <c r="D33">
+        <v>5</v>
+      </c>
+      <c r="E33">
+        <v>4191.7677928471803</v>
+      </c>
+      <c r="F33">
+        <v>10649.013058885599</v>
+      </c>
+      <c r="G33">
+        <v>4457.2452660384097</v>
+      </c>
+      <c r="H33">
+        <v>37</v>
+      </c>
+      <c r="I33" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J33" s="27">
+        <f t="shared" si="1"/>
+        <v>2.9135056836316453E-2</v>
+      </c>
+      <c r="K33" s="23">
+        <f t="shared" si="2"/>
+        <v>0.6166666666666667</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>82</v>
+      </c>
+      <c r="B34" s="25">
+        <v>4</v>
+      </c>
+      <c r="C34" s="25">
+        <v>3796</v>
+      </c>
+      <c r="D34">
+        <v>4</v>
+      </c>
+      <c r="E34">
+        <v>3807.6374022897799</v>
+      </c>
+      <c r="F34">
+        <v>8462.9743783879603</v>
+      </c>
+      <c r="G34">
+        <v>2655.33697609817</v>
+      </c>
+      <c r="H34">
+        <v>96</v>
+      </c>
+      <c r="I34" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J34" s="27">
+        <f t="shared" si="1"/>
+        <v>3.0663856691253155E-3</v>
+      </c>
+      <c r="K34" s="23">
+        <f t="shared" si="2"/>
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>121</v>
+      </c>
+      <c r="B35" s="25">
+        <v>4</v>
+      </c>
+      <c r="C35" s="25">
+        <v>3098.36</v>
+      </c>
+      <c r="D35">
+        <v>4</v>
+      </c>
+      <c r="E35">
+        <v>3106.8458963212902</v>
+      </c>
+      <c r="F35">
+        <v>8325.8621872933909</v>
+      </c>
+      <c r="G35">
+        <v>3219.0162909720998</v>
+      </c>
+      <c r="H35">
+        <v>247</v>
+      </c>
+      <c r="I35" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J35" s="27">
+        <f t="shared" si="1"/>
+        <v>2.7401593100866428E-3</v>
+      </c>
+      <c r="K35" s="23">
+        <f t="shared" si="2"/>
+        <v>4.1166666666666663</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>83</v>
+      </c>
+      <c r="B36" s="25">
+        <v>3</v>
+      </c>
+      <c r="C36" s="25">
+        <v>2486</v>
+      </c>
+      <c r="D36">
+        <v>3</v>
+      </c>
+      <c r="E36">
+        <v>2623.93108058699</v>
+      </c>
+      <c r="F36">
+        <v>6429.3242944153399</v>
+      </c>
+      <c r="G36">
+        <v>1805.3932138283401</v>
+      </c>
+      <c r="H36">
+        <v>554</v>
+      </c>
+      <c r="I36" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J36" s="27">
+        <f t="shared" si="1"/>
+        <v>5.5482703137570422E-2</v>
+      </c>
+      <c r="K36" s="23">
+        <f t="shared" si="2"/>
+        <v>9.2333333333333325</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>84</v>
+      </c>
+      <c r="B37" s="25">
+        <v>4</v>
+      </c>
+      <c r="C37" s="25">
+        <v>3438.39</v>
+      </c>
+      <c r="D37">
+        <v>4</v>
+      </c>
+      <c r="E37">
+        <v>3457.0542151218701</v>
+      </c>
+      <c r="F37">
+        <v>8478.1716270583402</v>
+      </c>
+      <c r="G37">
+        <v>3021.11741193646</v>
+      </c>
+      <c r="H37">
+        <v>133</v>
+      </c>
+      <c r="I37" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J37" s="27">
+        <f t="shared" si="1"/>
+        <v>5.4269585474597815E-3</v>
+      </c>
+      <c r="K37" s="23">
+        <f t="shared" si="2"/>
+        <v>2.2166666666666668</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>85</v>
+      </c>
+      <c r="B38" s="25">
+        <v>3</v>
+      </c>
+      <c r="C38" s="25">
+        <v>4457.95</v>
+      </c>
+      <c r="D38">
+        <v>4</v>
+      </c>
+      <c r="E38">
+        <v>3215.2060868096</v>
+      </c>
+      <c r="F38">
+        <v>8285.8472349959793</v>
+      </c>
+      <c r="G38">
+        <v>3070.6411481863702</v>
+      </c>
+      <c r="H38">
+        <v>492</v>
+      </c>
+      <c r="I38" s="27">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333326</v>
+      </c>
+      <c r="J38" s="27">
+        <f t="shared" si="1"/>
+        <v>-0.27876938951760333</v>
+      </c>
+      <c r="K38" s="23">
+        <f t="shared" si="2"/>
+        <v>8.1999999999999993</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>86</v>
+      </c>
+      <c r="B39" s="25">
+        <v>3</v>
+      </c>
+      <c r="C39" s="25">
+        <v>3098.35</v>
+      </c>
+      <c r="D39">
+        <v>4</v>
+      </c>
+      <c r="E39">
+        <v>2647.71627281468</v>
+      </c>
+      <c r="F39">
+        <v>8123.3443150804997</v>
+      </c>
+      <c r="G39">
+        <v>3475.6280422658101</v>
+      </c>
+      <c r="H39">
+        <v>807</v>
+      </c>
+      <c r="I39" s="27">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333326</v>
+      </c>
+      <c r="J39" s="27">
+        <f t="shared" si="1"/>
+        <v>-0.14544192876853812</v>
+      </c>
+      <c r="K39" s="23">
+        <f t="shared" si="2"/>
+        <v>13.45</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>87</v>
+      </c>
+      <c r="B40" s="25">
+        <v>2</v>
+      </c>
+      <c r="C40" s="25">
+        <v>2449.36</v>
+      </c>
+      <c r="D40">
+        <v>3</v>
+      </c>
+      <c r="E40">
+        <v>2149.23195358557</v>
+      </c>
+      <c r="F40">
+        <v>6069.8405387988196</v>
+      </c>
+      <c r="G40">
+        <v>1920.6085852132401</v>
+      </c>
+      <c r="H40">
+        <v>620</v>
+      </c>
+      <c r="I40" s="27">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="J40" s="27">
+        <f t="shared" si="1"/>
+        <v>-0.12253404971094495</v>
+      </c>
+      <c r="K40" s="23">
+        <f t="shared" si="2"/>
+        <v>10.333333333333334</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>88</v>
+      </c>
+      <c r="B41" s="25">
+        <v>3</v>
+      </c>
+      <c r="C41" s="25">
+        <v>3922.11</v>
+      </c>
+      <c r="D41">
+        <v>4</v>
+      </c>
+      <c r="E41">
+        <v>3198.4368311334101</v>
+      </c>
+      <c r="F41">
+        <v>8532.7417628602798</v>
+      </c>
+      <c r="G41">
+        <v>3334.3049317268601</v>
+      </c>
+      <c r="H41">
+        <v>135</v>
+      </c>
+      <c r="I41" s="27">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333326</v>
+      </c>
+      <c r="J41" s="27">
+        <f t="shared" si="1"/>
+        <v>-0.18451037834226991</v>
+      </c>
+      <c r="K41" s="23">
+        <f t="shared" si="2"/>
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>89</v>
+      </c>
+      <c r="B42" s="25">
+        <v>3</v>
+      </c>
+      <c r="C42" s="25">
+        <v>3254.83</v>
+      </c>
+      <c r="D42">
+        <v>3</v>
+      </c>
+      <c r="E42">
+        <v>3440.6486432656902</v>
+      </c>
+      <c r="F42">
+        <v>6308.2659055163303</v>
+      </c>
+      <c r="G42">
+        <v>867.61726225064103</v>
+      </c>
+      <c r="H42">
+        <v>385</v>
+      </c>
+      <c r="I42" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J42" s="27">
+        <f t="shared" si="1"/>
+        <v>5.7090539290838516E-2</v>
+      </c>
+      <c r="K42" s="23">
+        <f t="shared" si="2"/>
+        <v>6.416666666666667</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>122</v>
+      </c>
+      <c r="B43" s="25">
+        <v>19</v>
+      </c>
+      <c r="C43" s="25">
+        <v>3606.06</v>
+      </c>
+      <c r="D43">
+        <v>19</v>
+      </c>
+      <c r="E43">
+        <v>3606.0626270901998</v>
+      </c>
+      <c r="F43">
+        <v>8780.8145990318608</v>
+      </c>
+      <c r="G43">
+        <v>3174.75197194166</v>
+      </c>
+      <c r="H43">
+        <v>24</v>
+      </c>
+      <c r="I43" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J43" s="27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K43" s="23">
+        <f t="shared" si="2"/>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>90</v>
+      </c>
+      <c r="B44" s="25">
+        <v>15</v>
+      </c>
+      <c r="C44" s="25">
+        <v>3671.02</v>
+      </c>
+      <c r="D44">
+        <v>18</v>
+      </c>
+      <c r="E44">
+        <v>3314.3896682897798</v>
+      </c>
+      <c r="F44">
+        <v>8066.0887283747898</v>
+      </c>
+      <c r="G44">
+        <v>2751.6990600850099</v>
+      </c>
+      <c r="H44">
+        <v>40</v>
+      </c>
+      <c r="I44" s="27">
+        <f t="shared" si="0"/>
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="J44" s="27">
+        <f t="shared" si="1"/>
+        <v>-9.7147386829818494E-2</v>
+      </c>
+      <c r="K44" s="23">
+        <f t="shared" si="2"/>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>91</v>
+      </c>
+      <c r="B45" s="25">
+        <v>13</v>
+      </c>
+      <c r="C45" s="25">
+        <v>3154.92</v>
+      </c>
+      <c r="D45">
+        <v>14</v>
+      </c>
+      <c r="E45">
+        <v>3146.1924720734901</v>
+      </c>
+      <c r="F45">
+        <v>6657.9985092963498</v>
+      </c>
+      <c r="G45">
+        <v>1511.8060372228499</v>
+      </c>
+      <c r="H45">
+        <v>84</v>
+      </c>
+      <c r="I45" s="27">
+        <f t="shared" si="0"/>
+        <v>7.6923076923076872E-2</v>
+      </c>
+      <c r="J45" s="27">
+        <f t="shared" si="1"/>
+        <v>-2.7671066144308032E-3</v>
+      </c>
+      <c r="K45" s="23">
+        <f t="shared" si="2"/>
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>123</v>
+      </c>
+      <c r="B46" s="25">
+        <v>10</v>
+      </c>
+      <c r="C46" s="25">
+        <v>2631.82</v>
+      </c>
+      <c r="D46">
+        <v>10</v>
+      </c>
+      <c r="E46">
+        <v>2705.0625124431099</v>
+      </c>
+      <c r="F46">
+        <v>5658.2375743389002</v>
+      </c>
+      <c r="G46">
+        <v>953.17506189578603</v>
+      </c>
+      <c r="H46">
+        <v>324</v>
+      </c>
+      <c r="I46" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J46" s="27">
+        <f t="shared" si="1"/>
+        <v>2.7828650895577844E-2</v>
+      </c>
+      <c r="K46" s="23">
+        <f t="shared" si="2"/>
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>124</v>
+      </c>
+      <c r="B47" s="25">
+        <v>16</v>
+      </c>
+      <c r="C47" s="25">
+        <v>3715.81</v>
+      </c>
+      <c r="D47">
+        <v>16</v>
+      </c>
+      <c r="E47">
+        <v>3715.8301553852598</v>
+      </c>
+      <c r="F47">
+        <v>7641.0608703950302</v>
+      </c>
+      <c r="G47">
+        <v>1925.2307150097699</v>
+      </c>
+      <c r="H47">
+        <v>35</v>
+      </c>
+      <c r="I47" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J47" s="27">
+        <f t="shared" si="1"/>
+        <v>5.3824065278096356E-6</v>
+      </c>
+      <c r="K47" s="23">
+        <f t="shared" si="2"/>
+        <v>0.58333333333333337</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>92</v>
+      </c>
+      <c r="B48" s="25">
+        <v>16</v>
+      </c>
+      <c r="C48" s="25">
+        <v>3572.16</v>
+      </c>
+      <c r="D48">
+        <v>17</v>
+      </c>
+      <c r="E48">
+        <v>3368.7732082304101</v>
+      </c>
+      <c r="F48">
+        <v>7393.9618449593199</v>
+      </c>
+      <c r="G48">
+        <v>2025.1886367289101</v>
+      </c>
+      <c r="H48">
+        <v>49</v>
+      </c>
+      <c r="I48" s="27">
+        <f t="shared" si="0"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="J48" s="27">
+        <f t="shared" si="1"/>
+        <v>-5.6937539191973419E-2</v>
+      </c>
+      <c r="K48" s="23">
+        <f t="shared" si="2"/>
+        <v>0.81666666666666665</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>93</v>
+      </c>
+      <c r="B49" s="25">
+        <v>14</v>
+      </c>
+      <c r="C49" s="25">
+        <v>3666.34</v>
+      </c>
+      <c r="D49">
+        <v>16</v>
+      </c>
+      <c r="E49">
+        <v>3342.8166537427501</v>
+      </c>
+      <c r="F49">
+        <v>7036.7164418697303</v>
+      </c>
+      <c r="G49">
+        <v>1693.89978812697</v>
+      </c>
+      <c r="H49">
+        <v>44</v>
+      </c>
+      <c r="I49" s="27">
+        <f t="shared" si="0"/>
+        <v>0.14285714285714279</v>
+      </c>
+      <c r="J49" s="27">
+        <f t="shared" si="1"/>
+        <v>-8.8240588706993917E-2</v>
+      </c>
+      <c r="K49" s="23">
+        <f t="shared" si="2"/>
+        <v>0.73333333333333328</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>94</v>
+      </c>
+      <c r="B50" s="25">
+        <v>13</v>
+      </c>
+      <c r="C50" s="25">
+        <v>3145.74</v>
+      </c>
+      <c r="D50">
+        <v>14</v>
+      </c>
+      <c r="E50">
+        <v>3115.46044761754</v>
+      </c>
+      <c r="F50">
+        <v>6035.89474977174</v>
+      </c>
+      <c r="G50">
+        <v>920.43430215420904</v>
+      </c>
+      <c r="H50">
+        <v>49</v>
+      </c>
+      <c r="I50" s="27">
+        <f t="shared" si="0"/>
+        <v>7.6923076923076872E-2</v>
+      </c>
+      <c r="J50" s="27">
+        <f t="shared" si="1"/>
+        <v>-9.6257160477343229E-3</v>
+      </c>
+      <c r="K50" s="23">
+        <f t="shared" si="2"/>
+        <v>0.81666666666666665</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>95</v>
+      </c>
+      <c r="B51" s="25">
+        <v>13</v>
+      </c>
+      <c r="C51" s="25">
+        <v>3157.34</v>
+      </c>
+      <c r="D51">
+        <v>14</v>
+      </c>
+      <c r="E51">
+        <v>3204.5030179742098</v>
+      </c>
+      <c r="F51">
+        <v>6361.1871126878996</v>
+      </c>
+      <c r="G51">
+        <v>1156.68409471369</v>
+      </c>
+      <c r="H51">
+        <v>143</v>
+      </c>
+      <c r="I51" s="27">
+        <f t="shared" si="0"/>
+        <v>7.6923076923076872E-2</v>
+      </c>
+      <c r="J51" s="27">
+        <f t="shared" si="1"/>
+        <v>1.4936623866925958E-2</v>
+      </c>
+      <c r="K51" s="23">
+        <f t="shared" si="2"/>
+        <v>2.3833333333333333</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>96</v>
+      </c>
+      <c r="B52" s="25">
+        <v>12</v>
+      </c>
+      <c r="C52" s="25">
+        <v>2928.9</v>
+      </c>
+      <c r="D52">
+        <v>13</v>
+      </c>
+      <c r="E52">
+        <v>2862.2252200982098</v>
+      </c>
+      <c r="F52">
+        <v>5767.0071196553099</v>
+      </c>
+      <c r="G52">
+        <v>904.78189955710002</v>
+      </c>
+      <c r="H52">
+        <v>91</v>
+      </c>
+      <c r="I52" s="27">
+        <f t="shared" si="0"/>
+        <v>8.3333333333333259E-2</v>
+      </c>
+      <c r="J52" s="27">
+        <f t="shared" si="1"/>
+        <v>-2.2762811977192876E-2</v>
+      </c>
+      <c r="K52" s="23">
+        <f t="shared" si="2"/>
+        <v>1.5166666666666666</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>97</v>
+      </c>
+      <c r="B53" s="25">
+        <v>6</v>
+      </c>
+      <c r="C53" s="25">
+        <v>3595.18</v>
+      </c>
+      <c r="D53">
+        <v>7</v>
+      </c>
+      <c r="E53">
+        <v>2997.0563999368801</v>
+      </c>
+      <c r="F53">
+        <v>13700.2562968859</v>
+      </c>
+      <c r="G53">
+        <v>8703.1998969490396</v>
+      </c>
+      <c r="H53">
+        <v>98</v>
+      </c>
+      <c r="I53" s="27">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666674</v>
+      </c>
+      <c r="J53" s="27">
+        <f t="shared" si="1"/>
+        <v>-0.16636719162879188</v>
+      </c>
+      <c r="K53" s="23">
+        <f t="shared" si="2"/>
+        <v>1.6333333333333333</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>98</v>
+      </c>
+      <c r="B54" s="25">
+        <v>5</v>
+      </c>
+      <c r="C54" s="25">
+        <v>3158.25</v>
+      </c>
+      <c r="D54">
+        <v>6</v>
+      </c>
+      <c r="E54">
+        <v>2689.5540240371402</v>
+      </c>
+      <c r="F54">
+        <v>11319.8376768995</v>
+      </c>
+      <c r="G54">
+        <v>6630.2836528624102</v>
+      </c>
+      <c r="H54">
+        <v>175</v>
+      </c>
+      <c r="I54" s="27">
+        <f t="shared" si="0"/>
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="J54" s="27">
+        <f t="shared" si="1"/>
+        <v>-0.14840497110741702</v>
+      </c>
+      <c r="K54" s="23">
+        <f t="shared" si="2"/>
+        <v>2.9166666666666665</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>99</v>
+      </c>
+      <c r="B55" s="25">
+        <v>4</v>
+      </c>
+      <c r="C55" s="25">
+        <v>2881.99</v>
+      </c>
+      <c r="D55">
+        <v>5</v>
+      </c>
+      <c r="E55">
+        <v>2522.70011982608</v>
+      </c>
+      <c r="F55">
+        <v>8367.9603304346601</v>
+      </c>
+      <c r="G55">
+        <v>3845.2602106085801</v>
+      </c>
+      <c r="H55">
+        <v>449</v>
+      </c>
+      <c r="I55" s="27">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="J55" s="27">
+        <f t="shared" si="1"/>
+        <v>-0.12466733055978685</v>
+      </c>
+      <c r="K55" s="23">
+        <f t="shared" si="2"/>
+        <v>7.4833333333333334</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>100</v>
+      </c>
+      <c r="B56" s="25">
+        <v>3</v>
+      </c>
+      <c r="C56" s="25">
+        <v>2835.4</v>
+      </c>
+      <c r="D56">
+        <v>4</v>
+      </c>
+      <c r="E56">
+        <v>2415.5505691162598</v>
+      </c>
+      <c r="F56">
+        <v>6835.7704467039202</v>
+      </c>
+      <c r="G56">
+        <v>2420.21987758766</v>
+      </c>
+      <c r="H56">
+        <v>1067</v>
+      </c>
+      <c r="I56" s="27">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333326</v>
+      </c>
+      <c r="J56" s="27">
+        <f t="shared" si="1"/>
+        <v>-0.14807434577131973</v>
+      </c>
+      <c r="K56" s="23">
+        <f t="shared" si="2"/>
+        <v>17.783333333333335</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>125</v>
+      </c>
+      <c r="B57" s="25">
+        <v>5</v>
+      </c>
+      <c r="C57" s="25">
+        <v>2776.93</v>
+      </c>
+      <c r="D57">
+        <v>5</v>
+      </c>
+      <c r="E57">
+        <v>2832.7788223494099</v>
+      </c>
+      <c r="F57">
+        <v>9136.2218805541906</v>
+      </c>
+      <c r="G57">
+        <v>4303.4430582047798</v>
+      </c>
+      <c r="H57">
+        <v>66</v>
+      </c>
+      <c r="I57" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J57" s="27">
+        <f t="shared" si="1"/>
+        <v>2.0112138224586351E-2</v>
+      </c>
+      <c r="K57" s="23">
+        <f t="shared" si="2"/>
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>101</v>
+      </c>
+      <c r="B58" s="25">
+        <v>5</v>
+      </c>
+      <c r="C58" s="25">
+        <v>2707.96</v>
+      </c>
+      <c r="D58">
+        <v>5</v>
+      </c>
+      <c r="E58">
+        <v>2792.6908996847701</v>
+      </c>
+      <c r="F58">
+        <v>9863.8939775518993</v>
+      </c>
+      <c r="G58">
+        <v>5071.2030778671196</v>
+      </c>
+      <c r="H58">
+        <v>63</v>
+      </c>
+      <c r="I58" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J58" s="27">
+        <f t="shared" si="1"/>
+        <v>3.1289236177787005E-2</v>
+      </c>
+      <c r="K58" s="23">
+        <f t="shared" si="2"/>
+        <v>1.05</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>102</v>
+      </c>
+      <c r="B59" s="25">
+        <v>4</v>
+      </c>
+      <c r="C59" s="25">
+        <v>3010.68</v>
+      </c>
+      <c r="D59">
+        <v>5</v>
+      </c>
+      <c r="E59">
+        <v>2546.48027251344</v>
+      </c>
+      <c r="F59">
+        <v>9811.1333566392495</v>
+      </c>
+      <c r="G59">
+        <v>5264.6530841258</v>
+      </c>
+      <c r="H59">
+        <v>133</v>
+      </c>
+      <c r="I59" s="27">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="J59" s="27">
+        <f t="shared" si="1"/>
+        <v>-0.1541844367385441</v>
+      </c>
+      <c r="K59" s="23">
+        <f t="shared" si="2"/>
+        <v>2.2166666666666668</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>103</v>
+      </c>
+      <c r="B60" s="25">
+        <v>4</v>
+      </c>
+      <c r="C60" s="25">
+        <v>2399.89</v>
+      </c>
+      <c r="D60">
+        <v>4</v>
+      </c>
+      <c r="E60">
+        <v>2433.7019246392501</v>
+      </c>
+      <c r="F60">
+        <v>7720.6987746675404</v>
+      </c>
+      <c r="G60">
+        <v>3286.9968500282898</v>
+      </c>
+      <c r="H60">
+        <v>124</v>
+      </c>
+      <c r="I60" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J60" s="27">
+        <f t="shared" si="1"/>
+        <v>1.4088145706678157E-2</v>
+      </c>
+      <c r="K60" s="23">
+        <f t="shared" si="2"/>
+        <v>2.0666666666666669</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>126</v>
+      </c>
+      <c r="B61" s="25">
+        <v>4</v>
+      </c>
+      <c r="C61" s="25">
+        <v>2208.4899999999998</v>
+      </c>
+      <c r="D61">
+        <v>4</v>
+      </c>
+      <c r="E61">
+        <v>2234.8777379284302</v>
+      </c>
+      <c r="F61">
+        <v>7774.41182647188</v>
+      </c>
+      <c r="G61">
+        <v>3539.5340885434498</v>
+      </c>
+      <c r="H61">
+        <v>227</v>
+      </c>
+      <c r="I61" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J61" s="27">
+        <f t="shared" si="1"/>
+        <v>1.1949340952415621E-2</v>
+      </c>
+      <c r="K61" s="23">
+        <f t="shared" si="2"/>
+        <v>3.7833333333333332</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>104</v>
+      </c>
+      <c r="B62" s="25">
+        <v>3</v>
+      </c>
+      <c r="C62" s="25">
+        <v>2437.88</v>
+      </c>
+      <c r="D62">
+        <v>4</v>
+      </c>
+      <c r="E62">
+        <v>2105.6264295629599</v>
+      </c>
+      <c r="F62">
+        <v>7298.8363873850703</v>
+      </c>
+      <c r="G62">
+        <v>3193.2099578221</v>
+      </c>
+      <c r="H62">
+        <v>1158</v>
+      </c>
+      <c r="I62" s="27">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333326</v>
+      </c>
+      <c r="J62" s="27">
+        <f t="shared" si="1"/>
+        <v>-0.1362864456002757</v>
+      </c>
+      <c r="K62" s="23">
+        <f t="shared" si="2"/>
+        <v>19.3</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:H1"/>
+    <mergeCell ref="I1:K1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="I3:I62">
+    <cfRule type="cellIs" dxfId="3" priority="8" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3:I62">
+    <cfRule type="cellIs" dxfId="2" priority="7" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J3:J62">
+    <cfRule type="cellIs" dxfId="1" priority="5" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="6" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD41B92C-6AE7-414F-AF38-0F7EA59D03DF}">
+  <dimension ref="E3:E60"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C60"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="3" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E3" s="22"/>
+    </row>
+    <row r="4" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E4" s="22"/>
+    </row>
+    <row r="10" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E10" s="22"/>
+    </row>
+    <row r="22" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E22" s="22"/>
+    </row>
+    <row r="25" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E25" s="22"/>
+    </row>
+    <row r="29" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E29" s="22"/>
+    </row>
+    <row r="30" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E30" s="22"/>
+    </row>
+    <row r="33" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E33" s="22"/>
+    </row>
+    <row r="34" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E34" s="22"/>
+    </row>
+    <row r="36" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E36" s="22"/>
+    </row>
+    <row r="37" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E37" s="22"/>
+    </row>
+    <row r="38" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E38" s="22"/>
+    </row>
+    <row r="42" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E42" s="22"/>
+    </row>
+    <row r="44" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E44" s="22"/>
+    </row>
+    <row r="45" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E45" s="22"/>
+    </row>
+    <row r="46" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E46" s="22"/>
+    </row>
+    <row r="49" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E49" s="22"/>
+    </row>
+    <row r="50" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E50" s="22"/>
+    </row>
+    <row r="52" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E52" s="22"/>
+    </row>
+    <row r="53" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E53" s="22"/>
+    </row>
+    <row r="54" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E54" s="22"/>
+    </row>
+    <row r="55" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E55" s="22"/>
+    </row>
+    <row r="57" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E57" s="22"/>
+    </row>
+    <row r="58" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E58" s="22"/>
+    </row>
+    <row r="59" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E59" s="22"/>
+    </row>
+    <row r="60" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E60" s="22"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>